<commit_message>
feat: Basic mband.py working.
</commit_message>
<xml_diff>
--- a/Random/Matlab2025Files/SS/all_algorithm_metrics.xlsx
+++ b/Random/Matlab2025Files/SS/all_algorithm_metrics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\University\2025\Investigation\PROJECT-25P85\Random\Matlab2025Files\SS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E7440\Documents\Uni2025\Investigation\PROJECT-25P85\Random\Matlab2025Files\SS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3C5573-C604-47A3-8215-ECC385B12B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0031CC32-EFE3-4869-B788-B3CBE474A236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500"/>
+    <workbookView xWindow="990" yWindow="-120" windowWidth="19620" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,32 +20,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="286" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Algorithm</t>
   </si>
   <si>
-    <t>specsub_processed_output</t>
-  </si>
-  <si>
     <t>mband_processed_output</t>
   </si>
   <si>
+    <t>python_mband_processed_output</t>
+  </si>
+  <si>
     <t>File</t>
   </si>
   <si>
-    <t>specsub_sp21_station_sn0.wav</t>
-  </si>
-  <si>
-    <t>specsub_sp21_station_sn10.wav</t>
-  </si>
-  <si>
-    <t>specsub_sp21_station_sn15.wav</t>
-  </si>
-  <si>
-    <t>specsub_sp21_station_sn5.wav</t>
-  </si>
-  <si>
     <t>mband_sp21_station_sn0.wav</t>
   </si>
   <si>
@@ -58,6 +46,18 @@
     <t>mband_sp21_station_sn5.wav</t>
   </si>
   <si>
+    <t>python_mband_sp21_station_sn0.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn10.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn15.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn5.wav</t>
+  </si>
+  <si>
     <t>SNR</t>
   </si>
   <si>
@@ -125,28 +125,13 @@
   </si>
   <si>
     <t>SII</t>
-  </si>
-  <si>
-    <t>mband_causal_processed_output</t>
-  </si>
-  <si>
-    <t>mband_causal_sp21_station_sn0.wav</t>
-  </si>
-  <si>
-    <t>mband_causal_sp21_station_sn10.wav</t>
-  </si>
-  <si>
-    <t>mband_causal_sp21_station_sn15.wav</t>
-  </si>
-  <si>
-    <t>mband_causal_sp21_station_sn5.wav</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -194,7 +179,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -345,7 +330,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -369,9 +354,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -395,7 +380,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -430,7 +415,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -448,7 +433,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -473,7 +458,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -509,43 +494,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Y9"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="Y9" sqref="A1:Y9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.08984375" customWidth="true"/>
-    <col min="2" max="2" width="33.453125" customWidth="true"/>
-    <col min="3" max="3" width="12.08984375" customWidth="true"/>
-    <col min="5" max="5" width="11.453125" customWidth="true"/>
-    <col min="6" max="6" width="12.453125" customWidth="true"/>
-    <col min="7" max="7" width="11.453125" customWidth="true"/>
-    <col min="21" max="21" width="12.453125" customWidth="true"/>
-    <col min="24" max="24" width="13.453125" customWidth="true"/>
-    <col min="25" max="25" width="12.453125" customWidth="true"/>
-    <col min="4" max="4" width="12.08984375" customWidth="true"/>
-    <col min="8" max="8" width="11.453125" customWidth="true"/>
-    <col min="9" max="9" width="11.453125" customWidth="true"/>
-    <col min="10" max="10" width="11.453125" customWidth="true"/>
-    <col min="11" max="11" width="11.453125" customWidth="true"/>
-    <col min="12" max="12" width="11.453125" customWidth="true"/>
-    <col min="13" max="13" width="11.453125" customWidth="true"/>
-    <col min="14" max="14" width="11.453125" customWidth="true"/>
-    <col min="15" max="15" width="11.453125" customWidth="true"/>
-    <col min="16" max="16" width="11.453125" customWidth="true"/>
-    <col min="17" max="17" width="11.453125" customWidth="true"/>
-    <col min="18" max="18" width="11.453125" customWidth="true"/>
-    <col min="19" max="19" width="11.453125" customWidth="true"/>
-    <col min="20" max="20" width="11.453125" customWidth="true"/>
-    <col min="22" max="22" width="12.453125" customWidth="true"/>
-    <col min="23" max="23" width="12.453125" customWidth="true"/>
+    <col min="1" max="1" width="31.5703125" customWidth="true"/>
+    <col min="2" max="2" width="35.85546875" customWidth="true"/>
+    <col min="3" max="3" width="12.42578125" customWidth="true"/>
+    <col min="5" max="5" width="11.7109375" customWidth="true"/>
+    <col min="6" max="6" width="12.7109375" customWidth="true"/>
+    <col min="7" max="7" width="11.7109375" customWidth="true"/>
+    <col min="21" max="21" width="12.7109375" customWidth="true"/>
+    <col min="24" max="24" width="13.7109375" customWidth="true"/>
+    <col min="25" max="25" width="12.7109375" customWidth="true"/>
+    <col min="4" max="4" width="12.42578125" customWidth="true"/>
+    <col min="8" max="8" width="11.7109375" customWidth="true"/>
+    <col min="9" max="9" width="11.7109375" customWidth="true"/>
+    <col min="10" max="10" width="11.7109375" customWidth="true"/>
+    <col min="11" max="11" width="11.7109375" customWidth="true"/>
+    <col min="12" max="12" width="11.7109375" customWidth="true"/>
+    <col min="13" max="13" width="11.7109375" customWidth="true"/>
+    <col min="14" max="14" width="11.7109375" customWidth="true"/>
+    <col min="15" max="15" width="11.7109375" customWidth="true"/>
+    <col min="16" max="16" width="11.7109375" customWidth="true"/>
+    <col min="17" max="17" width="11.7109375" customWidth="true"/>
+    <col min="18" max="18" width="11.7109375" customWidth="true"/>
+    <col min="19" max="19" width="11.7109375" customWidth="true"/>
+    <col min="20" max="20" width="11.7109375" customWidth="true"/>
+    <col min="22" max="22" width="12.7109375" customWidth="true"/>
+    <col min="23" max="23" width="12.7109375" customWidth="true"/>
   </cols>
   <sheetData>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.35">
+    <row r="1">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -622,7 +607,7 @@
         <v>34</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
+    <row r="2">
       <c r="A2" s="0" t="s">
         <v>1</v>
       </c>
@@ -630,76 +615,76 @@
         <v>4</v>
       </c>
       <c r="C2" s="0">
-        <v>-4.4659674483216314</v>
+        <v>-10.206962587786265</v>
       </c>
       <c r="D2" s="0">
-        <v>-5.7667311340381113</v>
+        <v>-8.7632364591021208</v>
       </c>
       <c r="E2" s="0">
-        <v>87.546897311618722</v>
+        <v>80.383830439822262</v>
       </c>
       <c r="F2" s="0">
-        <v>1.0664662403220806</v>
+        <v>1.0774613457300257</v>
       </c>
       <c r="G2" s="0">
-        <v>3.0482103789829353</v>
+        <v>4.3070076111146811</v>
       </c>
       <c r="H2" s="0">
-        <v>6.1511307461536626</v>
+        <v>6.0293571045889687</v>
       </c>
       <c r="I2" s="0">
-        <v>6.0899897025491452</v>
+        <v>6.1429092773455816</v>
       </c>
       <c r="J2" s="0">
-        <v>2.6715947343929622</v>
+        <v>2.4296842457941334</v>
       </c>
       <c r="K2" s="0">
-        <v>2.2412760646676668</v>
+        <v>2.0364047570927508</v>
       </c>
       <c r="L2" s="0">
-        <v>2.2069913761700692</v>
+        <v>1.9628522693905692</v>
       </c>
       <c r="M2" s="0">
-        <v>2.7573395910522525</v>
+        <v>1.9796827468556308</v>
       </c>
       <c r="N2" s="0">
-        <v>1.950479573282333</v>
+        <v>2.1781637527108497</v>
       </c>
       <c r="O2" s="0">
-        <v>2.3320232121245601</v>
+        <v>1.9535190493745405</v>
       </c>
       <c r="P2" s="0">
-        <v>1.3946847928602675</v>
+        <v>1.8771836550370669</v>
       </c>
       <c r="Q2" s="0">
-        <v>1.281706051955934</v>
+        <v>1.5400311126230202</v>
       </c>
       <c r="R2" s="0">
-        <v>1.9063547533622498</v>
+        <v>2.2692155783666998</v>
       </c>
       <c r="S2" s="0">
-        <v>1.3245269883614759</v>
+        <v>1.4165230771055284</v>
       </c>
       <c r="T2" s="0">
-        <v>1.4870458753461149</v>
+        <v>1.9293040407605118</v>
       </c>
       <c r="U2" s="0">
-        <v>0.54101731377253826</v>
+        <v>0.55779137485575192</v>
       </c>
       <c r="V2" s="0">
-        <v>0.6041817762431323</v>
+        <v>0.63294303821523279</v>
       </c>
       <c r="W2" s="0">
-        <v>0.24275017889385633</v>
+        <v>0.36602415960328855</v>
       </c>
       <c r="X2" s="0">
-        <v>0.051559790372987788</v>
+        <v>0.047820163880449199</v>
       </c>
       <c r="Y2" s="0">
         <v>0.23571173354711331</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
+    <row r="3">
       <c r="A3" s="0" t="s">
         <v>1</v>
       </c>
@@ -707,76 +692,76 @@
         <v>5</v>
       </c>
       <c r="C3" s="0">
-        <v>-3.1495175833322269</v>
+        <v>-7.4920028083323125</v>
       </c>
       <c r="D3" s="0">
-        <v>-5.1077716015399384</v>
+        <v>-7.8958260986933926</v>
       </c>
       <c r="E3" s="0">
-        <v>61.943191795026124</v>
+        <v>56.276269303721904</v>
       </c>
       <c r="F3" s="0">
-        <v>0.64826639646350392</v>
+        <v>0.55717475663864435</v>
       </c>
       <c r="G3" s="0">
-        <v>1.810741985508747</v>
+        <v>2.1350521794214123</v>
       </c>
       <c r="H3" s="0">
-        <v>4.3918986327713654</v>
+        <v>4.060070898026269</v>
       </c>
       <c r="I3" s="0">
-        <v>11.286210207817712</v>
+        <v>11.002920887378444</v>
       </c>
       <c r="J3" s="0">
-        <v>4.608671338893422</v>
+        <v>4.3895344364072608</v>
       </c>
       <c r="K3" s="0">
-        <v>2.6708038199781816</v>
+        <v>2.7631765150699215</v>
       </c>
       <c r="L3" s="0">
-        <v>3.6003274614273386</v>
+        <v>3.5060319162816955</v>
       </c>
       <c r="M3" s="0">
-        <v>3.6091451446331941</v>
+        <v>3.8296044289359532</v>
       </c>
       <c r="N3" s="0">
-        <v>3.0751505501584138</v>
+        <v>3.009822587000814</v>
       </c>
       <c r="O3" s="0">
-        <v>3.0051379591974379</v>
+        <v>3.4441373781592137</v>
       </c>
       <c r="P3" s="0">
-        <v>2.5092552998093183</v>
+        <v>2.6152208136249246</v>
       </c>
       <c r="Q3" s="0">
-        <v>2.1464936052106305</v>
+        <v>2.2803227674681681</v>
       </c>
       <c r="R3" s="0">
-        <v>3.3732112717446352</v>
+        <v>3.590156149332298</v>
       </c>
       <c r="S3" s="0">
-        <v>2.0780320798466554</v>
+        <v>1.9927046195689764</v>
       </c>
       <c r="T3" s="0">
-        <v>2.8442985670590679</v>
+        <v>3.020044024647047</v>
       </c>
       <c r="U3" s="0">
-        <v>0.89644064663945322</v>
+        <v>0.89511970232695648</v>
       </c>
       <c r="V3" s="0">
-        <v>0.9358764550439822</v>
+        <v>0.93274279767632406</v>
       </c>
       <c r="W3" s="0">
-        <v>0.69226619019552138</v>
+        <v>0.69310217467735336</v>
       </c>
       <c r="X3" s="0">
-        <v>0.20493712323710009</v>
+        <v>0.22644291856792953</v>
       </c>
       <c r="Y3" s="0">
         <v>0.23571173354711331</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
+    <row r="4">
       <c r="A4" s="0" t="s">
         <v>1</v>
       </c>
@@ -784,76 +769,76 @@
         <v>6</v>
       </c>
       <c r="C4" s="0">
-        <v>-2.5765007322270557</v>
+        <v>-7.0988077885401148</v>
       </c>
       <c r="D4" s="0">
-        <v>-3.8048715638396997</v>
+        <v>-7.0983677765694786</v>
       </c>
       <c r="E4" s="0">
-        <v>47.375489681376976</v>
+        <v>40.725819242441403</v>
       </c>
       <c r="F4" s="0">
-        <v>0.45666143562275585</v>
+        <v>0.40229757303201485</v>
       </c>
       <c r="G4" s="0">
-        <v>1.7227197001265164</v>
+        <v>1.4532672881397013</v>
       </c>
       <c r="H4" s="0">
-        <v>3.4074691880585846</v>
+        <v>3.2756878352647587</v>
       </c>
       <c r="I4" s="0">
-        <v>13.68925331872132</v>
+        <v>12.851029913116449</v>
       </c>
       <c r="J4" s="0">
-        <v>5</v>
+        <v>4.6490308268226981</v>
       </c>
       <c r="K4" s="0">
-        <v>2.9680346106058586</v>
+        <v>3.0183892412638982</v>
       </c>
       <c r="L4" s="0">
-        <v>4.0805010078897634</v>
+        <v>3.770397652546162</v>
       </c>
       <c r="M4" s="0">
-        <v>3.9847308717425514</v>
+        <v>3.5604553026326329</v>
       </c>
       <c r="N4" s="0">
-        <v>3.2398310409675832</v>
+        <v>1.5382947017664645</v>
       </c>
       <c r="O4" s="0">
-        <v>3.4649482707509622</v>
+        <v>4.1017506483269415</v>
       </c>
       <c r="P4" s="0">
-        <v>2.9279803769446358</v>
+        <v>3.0112614726900464</v>
       </c>
       <c r="Q4" s="0">
-        <v>2.7160768884776103</v>
+        <v>2.838973094345131</v>
       </c>
       <c r="R4" s="0">
-        <v>3.962288142909407</v>
+        <v>4.1282940922001821</v>
       </c>
       <c r="S4" s="0">
-        <v>2.4622392838879961</v>
+        <v>2.3411050793248749</v>
       </c>
       <c r="T4" s="0">
-        <v>3.3855851206319425</v>
+        <v>3.5270083934260059</v>
       </c>
       <c r="U4" s="0">
-        <v>0.94125592753470599</v>
+        <v>0.94336477866728841</v>
       </c>
       <c r="V4" s="0">
-        <v>0.98548438880007727</v>
+        <v>0.98303586609633664</v>
       </c>
       <c r="W4" s="0">
-        <v>0.85906884603635014</v>
+        <v>0.85278164553633851</v>
       </c>
       <c r="X4" s="0">
-        <v>0.27092694704284653</v>
+        <v>0.30246232820655033</v>
       </c>
       <c r="Y4" s="0">
         <v>0.23571173354711331</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
+    <row r="5">
       <c r="A5" s="0" t="s">
         <v>1</v>
       </c>
@@ -861,76 +846,76 @@
         <v>7</v>
       </c>
       <c r="C5" s="0">
-        <v>-5.3101667584835326</v>
+        <v>-9.1155293751566155</v>
       </c>
       <c r="D5" s="0">
-        <v>-6.9013660779438712</v>
+        <v>-8.8648797560871735</v>
       </c>
       <c r="E5" s="0">
-        <v>64.558581916861385</v>
+        <v>58.720542706425235</v>
       </c>
       <c r="F5" s="0">
-        <v>0.72727546219642614</v>
+        <v>0.7249952104412537</v>
       </c>
       <c r="G5" s="0">
-        <v>2.3812777801461702</v>
+        <v>2.9412518374919721</v>
       </c>
       <c r="H5" s="0">
-        <v>4.9486902872213285</v>
+        <v>4.9929053340945995</v>
       </c>
       <c r="I5" s="0">
-        <v>8.8201382802024302</v>
+        <v>8.6172338883876449</v>
       </c>
       <c r="J5" s="0">
-        <v>4.1371990890810757</v>
+        <v>3.994858507289675</v>
       </c>
       <c r="K5" s="0">
-        <v>2.2445497189112795</v>
+        <v>2.4224201164402768</v>
       </c>
       <c r="L5" s="0">
-        <v>3.1144200669236057</v>
+        <v>3.1216152348072068</v>
       </c>
       <c r="M5" s="0">
-        <v>3.1104628942222616</v>
+        <v>3.2813624654715969</v>
       </c>
       <c r="N5" s="0">
-        <v>2.3971770825547409</v>
+        <v>2.6421734865610143</v>
       </c>
       <c r="O5" s="0">
-        <v>2.6154549182819342</v>
+        <v>2.7223095967364173</v>
       </c>
       <c r="P5" s="0">
-        <v>2.4465480482812483</v>
+        <v>2.4369790533194928</v>
       </c>
       <c r="Q5" s="0">
-        <v>2.0713606818236485</v>
+        <v>2.0601736371841146</v>
       </c>
       <c r="R5" s="0">
-        <v>3.226530330191923</v>
+        <v>3.2742951051865758</v>
       </c>
       <c r="S5" s="0">
-        <v>1.916753830749943</v>
+        <v>1.829344763908249</v>
       </c>
       <c r="T5" s="0">
-        <v>2.7330538326563465</v>
+        <v>2.7667109178315274</v>
       </c>
       <c r="U5" s="0">
-        <v>0.77053293921729005</v>
+        <v>0.77154919263139143</v>
       </c>
       <c r="V5" s="0">
-        <v>0.8398143980938263</v>
+        <v>0.83653851376018207</v>
       </c>
       <c r="W5" s="0">
-        <v>0.57348178129632477</v>
+        <v>0.56994932531555342</v>
       </c>
       <c r="X5" s="0">
-        <v>0.15744986654118256</v>
+        <v>0.16371209276939594</v>
       </c>
       <c r="Y5" s="0">
         <v>0.23571173354711331</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
+    <row r="6">
       <c r="A6" s="0" t="s">
         <v>2</v>
       </c>
@@ -938,76 +923,76 @@
         <v>8</v>
       </c>
       <c r="C6" s="0">
-        <v>-8.5485798740429075</v>
+        <v>-5.4256534416546103</v>
       </c>
       <c r="D6" s="0">
-        <v>-7.8186954769860115</v>
+        <v>-6.1252988909726689</v>
       </c>
       <c r="E6" s="0">
-        <v>76.115569507737561</v>
+        <v>82.395763382743425</v>
       </c>
       <c r="F6" s="0">
-        <v>1.0637284526118578</v>
+        <v>1.2524010760382598</v>
       </c>
       <c r="G6" s="0">
-        <v>3.7012699802074374</v>
+        <v>3.3605203219881514</v>
       </c>
       <c r="H6" s="0">
-        <v>6.0933217976940091</v>
+        <v>6.7307862537487537</v>
       </c>
       <c r="I6" s="0">
-        <v>6.0503894393303073</v>
+        <v>5.6112459365503025</v>
       </c>
       <c r="J6" s="0">
-        <v>2.364772527758932</v>
+        <v>2.188689275084541</v>
       </c>
       <c r="K6" s="0">
-        <v>2.0302092899651214</v>
+        <v>1.8827382764360228</v>
       </c>
       <c r="L6" s="0">
-        <v>1.9419944169125303</v>
+        <v>1.7531948422383228</v>
       </c>
       <c r="M6" s="0">
-        <v>2.1530192012362019</v>
+        <v>2.1521715376724111</v>
       </c>
       <c r="N6" s="0">
-        <v>2.090847134109556</v>
+        <v>2.1263487994251453</v>
       </c>
       <c r="O6" s="0">
-        <v>2.1658217118195751</v>
+        <v>2.1638609081904012</v>
       </c>
       <c r="P6" s="0">
-        <v>1.8761890347670953</v>
+        <v>1.8195105822837523</v>
       </c>
       <c r="Q6" s="0">
-        <v>1.5393360456542964</v>
+        <v>1.500958340962717</v>
       </c>
       <c r="R6" s="0">
-        <v>2.3333275224678585</v>
+        <v>1.7975047007915141</v>
       </c>
       <c r="S6" s="0">
-        <v>1.5054315570143899</v>
+        <v>1.541061884521151</v>
       </c>
       <c r="T6" s="0">
-        <v>1.97146598328208</v>
+        <v>1.6603979348658058</v>
       </c>
       <c r="U6" s="0">
-        <v>0.56268936367670208</v>
+        <v>0.55460607953434693</v>
       </c>
       <c r="V6" s="0">
-        <v>0.6502012509918863</v>
+        <v>0.64592956314178585</v>
       </c>
       <c r="W6" s="0">
-        <v>0.37607084722408091</v>
+        <v>0.35524338065101529</v>
       </c>
       <c r="X6" s="0">
-        <v>0.040314128773576173</v>
+        <v>0.055756942754893526</v>
       </c>
       <c r="Y6" s="0">
         <v>0.23571173354711331</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.35">
+    <row r="7">
       <c r="A7" s="0" t="s">
         <v>2</v>
       </c>
@@ -1015,76 +1000,76 @@
         <v>9</v>
       </c>
       <c r="C7" s="0">
-        <v>-6.3772198878785193</v>
+        <v>-2.2829037278246589</v>
       </c>
       <c r="D7" s="0">
-        <v>-7.1241338228082833</v>
+        <v>-4.6356745171806635</v>
       </c>
       <c r="E7" s="0">
-        <v>51.26140278009035</v>
+        <v>58.251562748310889</v>
       </c>
       <c r="F7" s="0">
-        <v>0.60674509297341872</v>
+        <v>0.61049017437337472</v>
       </c>
       <c r="G7" s="0">
-        <v>1.8198975576403747</v>
+        <v>1.6520715554956062</v>
       </c>
       <c r="H7" s="0">
-        <v>4.2944577880489368</v>
+        <v>4.228667787795132</v>
       </c>
       <c r="I7" s="0">
-        <v>10.517490430560629</v>
+        <v>10.465388017775483</v>
       </c>
       <c r="J7" s="0">
-        <v>3.9581710288706606</v>
+        <v>4.1287548074654721</v>
       </c>
       <c r="K7" s="0">
-        <v>2.8901025888258571</v>
+        <v>2.758219547345699</v>
       </c>
       <c r="L7" s="0">
-        <v>3.3218757092161067</v>
+        <v>3.3312401648869954</v>
       </c>
       <c r="M7" s="0">
-        <v>3.9149568210124843</v>
+        <v>3.9404560946225091</v>
       </c>
       <c r="N7" s="0">
-        <v>3.450985516073886</v>
+        <v>3.2316942259320962</v>
       </c>
       <c r="O7" s="0">
-        <v>3.4846402687314999</v>
+        <v>3.4582496123785496</v>
       </c>
       <c r="P7" s="0">
-        <v>2.601772396032449</v>
+        <v>2.6530800084833936</v>
       </c>
       <c r="Q7" s="0">
-        <v>2.2628828960183851</v>
+        <v>2.3300900591311646</v>
       </c>
       <c r="R7" s="0">
-        <v>3.574492909694881</v>
+        <v>3.5376054459958071</v>
       </c>
       <c r="S7" s="0">
-        <v>2.0699969550059567</v>
+        <v>2.2023638102345036</v>
       </c>
       <c r="T7" s="0">
-        <v>3.0181062997856847</v>
+        <v>3.0080324909096543</v>
       </c>
       <c r="U7" s="0">
-        <v>0.90158334741169344</v>
+        <v>0.88318398615720983</v>
       </c>
       <c r="V7" s="0">
-        <v>0.90841098611064308</v>
+        <v>0.91143754895911311</v>
       </c>
       <c r="W7" s="0">
-        <v>0.68496878593128507</v>
+        <v>0.68549928160878848</v>
       </c>
       <c r="X7" s="0">
-        <v>0.20817752525871697</v>
+        <v>0.19218256213792426</v>
       </c>
       <c r="Y7" s="0">
         <v>0.23571173354711331</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
+    <row r="8">
       <c r="A8" s="0" t="s">
         <v>2</v>
       </c>
@@ -1092,76 +1077,76 @@
         <v>10</v>
       </c>
       <c r="C8" s="0">
-        <v>-6.0382867568486684</v>
+        <v>-1.6799527745454543</v>
       </c>
       <c r="D8" s="0">
-        <v>-6.5129714901912914</v>
+        <v>-3.2618109241522348</v>
       </c>
       <c r="E8" s="0">
-        <v>40.359746677123141</v>
+        <v>42.561159165676656</v>
       </c>
       <c r="F8" s="0">
-        <v>0.42506162981666107</v>
+        <v>0.42608812538636798</v>
       </c>
       <c r="G8" s="0">
-        <v>1.4661518813452557</v>
+        <v>1.3977784009543981</v>
       </c>
       <c r="H8" s="0">
-        <v>3.4682183225852263</v>
+        <v>3.3738519076660829</v>
       </c>
       <c r="I8" s="0">
-        <v>12.03598930935105</v>
+        <v>12.104287877743539</v>
       </c>
       <c r="J8" s="0">
-        <v>4.1648031588382786</v>
+        <v>4.5327240209635695</v>
       </c>
       <c r="K8" s="0">
-        <v>2.9484716317121285</v>
+        <v>2.9085473771283366</v>
       </c>
       <c r="L8" s="0">
-        <v>3.4617709445197717</v>
+        <v>3.661451088994732</v>
       </c>
       <c r="M8" s="0">
-        <v>3.8307356378113382</v>
+        <v>3.8333142723690998</v>
       </c>
       <c r="N8" s="0">
-        <v>1.4533504735832592</v>
+        <v>1.7623678220112398</v>
       </c>
       <c r="O8" s="0">
-        <v>3.8113180359322367</v>
+        <v>3.8267200343308083</v>
       </c>
       <c r="P8" s="0">
-        <v>2.9820199420242166</v>
+        <v>3.1010535902591347</v>
       </c>
       <c r="Q8" s="0">
-        <v>2.7956340793634826</v>
+        <v>2.9728260850511794</v>
       </c>
       <c r="R8" s="0">
-        <v>4.0905318878651498</v>
+        <v>4.1414402014125953</v>
       </c>
       <c r="S8" s="0">
-        <v>2.366570101665662</v>
+        <v>2.6128814137625387</v>
       </c>
       <c r="T8" s="0">
-        <v>3.4943762721235014</v>
+        <v>3.5742629058010467</v>
       </c>
       <c r="U8" s="0">
-        <v>0.93748530758554904</v>
+        <v>0.92678861703500937</v>
       </c>
       <c r="V8" s="0">
-        <v>0.95337751966252382</v>
+        <v>0.96069931422446331</v>
       </c>
       <c r="W8" s="0">
-        <v>0.82497581497185257</v>
+        <v>0.82645053025151838</v>
       </c>
       <c r="X8" s="0">
-        <v>0.28214594634898915</v>
+        <v>0.27557459216999963</v>
       </c>
       <c r="Y8" s="0">
         <v>0.23571173354711331</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
+    <row r="9">
       <c r="A9" s="0" t="s">
         <v>2</v>
       </c>
@@ -1169,380 +1154,72 @@
         <v>11</v>
       </c>
       <c r="C9" s="0">
-        <v>-8.025338879250711</v>
+        <v>-4.4471840550030661</v>
       </c>
       <c r="D9" s="0">
-        <v>-8.4549570367357632</v>
+        <v>-6.4276712845226314</v>
       </c>
       <c r="E9" s="0">
-        <v>59.087109840062261</v>
+        <v>62.695226982427926</v>
       </c>
       <c r="F9" s="0">
-        <v>0.77350611996255514</v>
+        <v>0.74201775806471393</v>
       </c>
       <c r="G9" s="0">
-        <v>2.716537229351538</v>
+        <v>2.2406447635894335</v>
       </c>
       <c r="H9" s="0">
-        <v>5.1631338718877746</v>
+        <v>5.0158698967966151</v>
       </c>
       <c r="I9" s="0">
-        <v>8.2342659036933163</v>
+        <v>8.0959689444999619</v>
       </c>
       <c r="J9" s="0">
-        <v>3.6560280516966834</v>
+        <v>3.6704823493522802</v>
       </c>
       <c r="K9" s="0">
-        <v>2.2935280482498976</v>
+        <v>2.3209325211337659</v>
       </c>
       <c r="L9" s="0">
-        <v>2.8615516141641204</v>
+        <v>2.869428061557715</v>
       </c>
       <c r="M9" s="0">
-        <v>3.4292117573950893</v>
+        <v>3.4050393814484843</v>
       </c>
       <c r="N9" s="0">
-        <v>2.8938529170377203</v>
+        <v>2.7230306232554295</v>
       </c>
       <c r="O9" s="0">
-        <v>2.8330499803292888</v>
+        <v>2.8230520740093228</v>
       </c>
       <c r="P9" s="0">
-        <v>2.4443287998607275</v>
+        <v>2.4513979278147717</v>
       </c>
       <c r="Q9" s="0">
-        <v>2.0687595282970013</v>
+        <v>2.0770590965654714</v>
       </c>
       <c r="R9" s="0">
-        <v>3.223107946956616</v>
+        <v>3.225888985923258</v>
       </c>
       <c r="S9" s="0">
-        <v>1.8561171041386388</v>
+        <v>1.9619583296935392</v>
       </c>
       <c r="T9" s="0">
-        <v>2.7440286318500084</v>
+        <v>2.7398828694336381</v>
       </c>
       <c r="U9" s="0">
-        <v>0.77316881395976445</v>
+        <v>0.75944126355599784</v>
       </c>
       <c r="V9" s="0">
-        <v>0.81599283138694234</v>
+        <v>0.81779930659885325</v>
       </c>
       <c r="W9" s="0">
-        <v>0.57099320667547016</v>
+        <v>0.56577424903760243</v>
       </c>
       <c r="X9" s="0">
-        <v>0.16026574709830702</v>
+        <v>0.14366901585684408</v>
       </c>
       <c r="Y9" s="0">
-        <v>0.23571173354711331</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="0">
-        <v>-7.564351881118176</v>
-      </c>
-      <c r="D10" s="0">
-        <v>-6.9711547619170871</v>
-      </c>
-      <c r="E10" s="0">
-        <v>82.124213112312319</v>
-      </c>
-      <c r="F10" s="0">
-        <v>1.1960303941002033</v>
-      </c>
-      <c r="G10" s="0">
-        <v>4.138158688078474</v>
-      </c>
-      <c r="H10" s="0">
-        <v>6.3527646303669369</v>
-      </c>
-      <c r="I10" s="0">
-        <v>4.9386593569440791</v>
-      </c>
-      <c r="J10" s="0">
-        <v>1.8666298694153691</v>
-      </c>
-      <c r="K10" s="0">
-        <v>1.777129930159866</v>
-      </c>
-      <c r="L10" s="0">
-        <v>1.5347929672620837</v>
-      </c>
-      <c r="M10" s="0">
-        <v>1</v>
-      </c>
-      <c r="N10" s="0">
-        <v>2.1747065015762748</v>
-      </c>
-      <c r="O10" s="0">
-        <v>1.1520978677396283</v>
-      </c>
-      <c r="P10" s="0">
-        <v>2.1618597945041653</v>
-      </c>
-      <c r="Q10" s="0">
-        <v>1.7715190590547558</v>
-      </c>
-      <c r="R10" s="0">
-        <v>2.2687928171466245</v>
-      </c>
-      <c r="S10" s="0">
-        <v>1.6533167399860276</v>
-      </c>
-      <c r="T10" s="0">
-        <v>2.0684561664870129</v>
-      </c>
-      <c r="U10" s="0">
-        <v>0.39207329527565199</v>
-      </c>
-      <c r="V10" s="0">
-        <v>0.51894466460790079</v>
-      </c>
-      <c r="W10" s="0">
-        <v>0.30530502113840891</v>
-      </c>
-      <c r="X10" s="0">
-        <v>0.043271164584995102</v>
-      </c>
-      <c r="Y10" s="0">
-        <v>0.23571173354711331</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="0">
-        <v>-4.4845321985318929</v>
-      </c>
-      <c r="D11" s="0">
-        <v>-5.7568088704627813</v>
-      </c>
-      <c r="E11" s="0">
-        <v>53.527513705250733</v>
-      </c>
-      <c r="F11" s="0">
-        <v>0.72358724980250411</v>
-      </c>
-      <c r="G11" s="0">
-        <v>2.5099908196570384</v>
-      </c>
-      <c r="H11" s="0">
-        <v>4.6978362685580688</v>
-      </c>
-      <c r="I11" s="0">
-        <v>7.9216459445005336</v>
-      </c>
-      <c r="J11" s="0">
-        <v>3.2044801729379948</v>
-      </c>
-      <c r="K11" s="0">
-        <v>2.4818268028528108</v>
-      </c>
-      <c r="L11" s="0">
-        <v>2.6825595293100815</v>
-      </c>
-      <c r="M11" s="0">
-        <v>3.4493642042760921</v>
-      </c>
-      <c r="N11" s="0">
-        <v>2.8706571060312456</v>
-      </c>
-      <c r="O11" s="0">
-        <v>2.7495647569846202</v>
-      </c>
-      <c r="P11" s="0">
-        <v>2.0824257258184238</v>
-      </c>
-      <c r="Q11" s="0">
-        <v>1.7002035501512305</v>
-      </c>
-      <c r="R11" s="0">
-        <v>3.1223838092744765</v>
-      </c>
-      <c r="S11" s="0">
-        <v>1.8920279421652964</v>
-      </c>
-      <c r="T11" s="0">
-        <v>2.5251834414481942</v>
-      </c>
-      <c r="U11" s="0">
-        <v>0.58199595447901953</v>
-      </c>
-      <c r="V11" s="0">
-        <v>0.69578034963010427</v>
-      </c>
-      <c r="W11" s="0">
-        <v>0.52040642352054112</v>
-      </c>
-      <c r="X11" s="0">
-        <v>0.16455493890718848</v>
-      </c>
-      <c r="Y11" s="0">
-        <v>0.23571173354711331</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="0">
-        <v>-3.5780616939775287</v>
-      </c>
-      <c r="D12" s="0">
-        <v>-5.1145887673906945</v>
-      </c>
-      <c r="E12" s="0">
-        <v>50.84355739772235</v>
-      </c>
-      <c r="F12" s="0">
-        <v>0.64976254149665214</v>
-      </c>
-      <c r="G12" s="0">
-        <v>2.0637111280240807</v>
-      </c>
-      <c r="H12" s="0">
-        <v>4.6997471127597121</v>
-      </c>
-      <c r="I12" s="0">
-        <v>7.7819427162756458</v>
-      </c>
-      <c r="J12" s="0">
-        <v>2.7628336649794223</v>
-      </c>
-      <c r="K12" s="0">
-        <v>2.2840267912397936</v>
-      </c>
-      <c r="L12" s="0">
-        <v>2.3192994672923009</v>
-      </c>
-      <c r="M12" s="0">
-        <v>3.0752239060350433</v>
-      </c>
-      <c r="N12" s="0">
-        <v>2.6288763433282711</v>
-      </c>
-      <c r="O12" s="0">
-        <v>2.3189211563516175</v>
-      </c>
-      <c r="P12" s="0">
-        <v>2.3281615246451031</v>
-      </c>
-      <c r="Q12" s="0">
-        <v>1.9383010123564777</v>
-      </c>
-      <c r="R12" s="0">
-        <v>3.370683727581441</v>
-      </c>
-      <c r="S12" s="0">
-        <v>2.0687372146506888</v>
-      </c>
-      <c r="T12" s="0">
-        <v>2.7795867043089659</v>
-      </c>
-      <c r="U12" s="0">
-        <v>0.59611031034921047</v>
-      </c>
-      <c r="V12" s="0">
-        <v>0.72210352811706868</v>
-      </c>
-      <c r="W12" s="0">
-        <v>0.56556987333239761</v>
-      </c>
-      <c r="X12" s="0">
-        <v>0.21437954274361659</v>
-      </c>
-      <c r="Y12" s="0">
-        <v>0.23571173354711331</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="0">
-        <v>-6.2663155656196254</v>
-      </c>
-      <c r="D13" s="0">
-        <v>-7.1685294531323578</v>
-      </c>
-      <c r="E13" s="0">
-        <v>47.810108956936681</v>
-      </c>
-      <c r="F13" s="0">
-        <v>0.81921040570368176</v>
-      </c>
-      <c r="G13" s="0">
-        <v>3.1661255916720972</v>
-      </c>
-      <c r="H13" s="0">
-        <v>5.3793746239889515</v>
-      </c>
-      <c r="I13" s="0">
-        <v>6.6286027896804116</v>
-      </c>
-      <c r="J13" s="0">
-        <v>2.9894030353725842</v>
-      </c>
-      <c r="K13" s="0">
-        <v>2.0604954011136067</v>
-      </c>
-      <c r="L13" s="0">
-        <v>2.3721778380135938</v>
-      </c>
-      <c r="M13" s="0">
-        <v>3.0399559020489351</v>
-      </c>
-      <c r="N13" s="0">
-        <v>2.2751197741667522</v>
-      </c>
-      <c r="O13" s="0">
-        <v>2.0972434004067653</v>
-      </c>
-      <c r="P13" s="0">
-        <v>2.0236883026665229</v>
-      </c>
-      <c r="Q13" s="0">
-        <v>1.6508777877957428</v>
-      </c>
-      <c r="R13" s="0">
-        <v>3.0346219061403894</v>
-      </c>
-      <c r="S13" s="0">
-        <v>1.8150348904287024</v>
-      </c>
-      <c r="T13" s="0">
-        <v>2.466273895491621</v>
-      </c>
-      <c r="U13" s="0">
-        <v>0.54069547484599312</v>
-      </c>
-      <c r="V13" s="0">
-        <v>0.65732445104704063</v>
-      </c>
-      <c r="W13" s="0">
-        <v>0.48557333456103247</v>
-      </c>
-      <c r="X13" s="0">
-        <v>0.11906293045249729</v>
-      </c>
-      <c r="Y13" s="0">
         <v>0.23571173354711331</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Mband with some additional real-time modifications as well as deltas
</commit_message>
<xml_diff>
--- a/Random/Matlab2025Files/SS/all_algorithm_metrics.xlsx
+++ b/Random/Matlab2025Files/SS/all_algorithm_metrics.xlsx
@@ -20,7 +20,637 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="245">
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>mband_processed_output</t>
+  </si>
+  <si>
+    <t>python_mband_processed_output</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>mband_sp21_station_sn0.wav</t>
+  </si>
+  <si>
+    <t>mband_sp21_station_sn10.wav</t>
+  </si>
+  <si>
+    <t>mband_sp21_station_sn15.wav</t>
+  </si>
+  <si>
+    <t>mband_sp21_station_sn5.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn0.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn10.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn15.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn5.wav</t>
+  </si>
+  <si>
+    <t>SNR</t>
+  </si>
+  <si>
+    <t>SegSNR</t>
+  </si>
+  <si>
+    <t>WSS</t>
+  </si>
+  <si>
+    <t>LLR</t>
+  </si>
+  <si>
+    <t>IS</t>
+  </si>
+  <si>
+    <t>CEP</t>
+  </si>
+  <si>
+    <t>fwSNRseg</t>
+  </si>
+  <si>
+    <t>SIGv</t>
+  </si>
+  <si>
+    <t>BAKv</t>
+  </si>
+  <si>
+    <t>OVLv</t>
+  </si>
+  <si>
+    <t>SIGm</t>
+  </si>
+  <si>
+    <t>BAKm</t>
+  </si>
+  <si>
+    <t>OVLm</t>
+  </si>
+  <si>
+    <t>PESQ_1</t>
+  </si>
+  <si>
+    <t>PESQ_2</t>
+  </si>
+  <si>
+    <t>Csig</t>
+  </si>
+  <si>
+    <t>Cbak</t>
+  </si>
+  <si>
+    <t>Covl</t>
+  </si>
+  <si>
+    <t>NCM</t>
+  </si>
+  <si>
+    <t>CSh</t>
+  </si>
+  <si>
+    <t>CSm</t>
+  </si>
+  <si>
+    <t>CSl</t>
+  </si>
+  <si>
+    <t>SII</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>mband_processed_output</t>
+  </si>
+  <si>
+    <t>python_mband_processed_output</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>mband_sp21_station_sn0.wav</t>
+  </si>
+  <si>
+    <t>mband_sp21_station_sn10.wav</t>
+  </si>
+  <si>
+    <t>mband_sp21_station_sn15.wav</t>
+  </si>
+  <si>
+    <t>mband_sp21_station_sn5.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn0.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn10.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn15.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn5.wav</t>
+  </si>
+  <si>
+    <t>SNR</t>
+  </si>
+  <si>
+    <t>SegSNR</t>
+  </si>
+  <si>
+    <t>WSS</t>
+  </si>
+  <si>
+    <t>LLR</t>
+  </si>
+  <si>
+    <t>IS</t>
+  </si>
+  <si>
+    <t>CEP</t>
+  </si>
+  <si>
+    <t>fwSNRseg</t>
+  </si>
+  <si>
+    <t>SIGv</t>
+  </si>
+  <si>
+    <t>BAKv</t>
+  </si>
+  <si>
+    <t>OVLv</t>
+  </si>
+  <si>
+    <t>SIGm</t>
+  </si>
+  <si>
+    <t>BAKm</t>
+  </si>
+  <si>
+    <t>OVLm</t>
+  </si>
+  <si>
+    <t>PESQ_1</t>
+  </si>
+  <si>
+    <t>PESQ_2</t>
+  </si>
+  <si>
+    <t>Csig</t>
+  </si>
+  <si>
+    <t>Cbak</t>
+  </si>
+  <si>
+    <t>Covl</t>
+  </si>
+  <si>
+    <t>NCM</t>
+  </si>
+  <si>
+    <t>CSh</t>
+  </si>
+  <si>
+    <t>CSm</t>
+  </si>
+  <si>
+    <t>CSl</t>
+  </si>
+  <si>
+    <t>SII</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>mband_processed_output</t>
+  </si>
+  <si>
+    <t>python_mband_processed_output</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>mband_sp21_station_sn0.wav</t>
+  </si>
+  <si>
+    <t>mband_sp21_station_sn10.wav</t>
+  </si>
+  <si>
+    <t>mband_sp21_station_sn15.wav</t>
+  </si>
+  <si>
+    <t>mband_sp21_station_sn5.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn0.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn10.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn15.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn5.wav</t>
+  </si>
+  <si>
+    <t>SNR</t>
+  </si>
+  <si>
+    <t>SegSNR</t>
+  </si>
+  <si>
+    <t>WSS</t>
+  </si>
+  <si>
+    <t>LLR</t>
+  </si>
+  <si>
+    <t>IS</t>
+  </si>
+  <si>
+    <t>CEP</t>
+  </si>
+  <si>
+    <t>fwSNRseg</t>
+  </si>
+  <si>
+    <t>SIGv</t>
+  </si>
+  <si>
+    <t>BAKv</t>
+  </si>
+  <si>
+    <t>OVLv</t>
+  </si>
+  <si>
+    <t>SIGm</t>
+  </si>
+  <si>
+    <t>BAKm</t>
+  </si>
+  <si>
+    <t>OVLm</t>
+  </si>
+  <si>
+    <t>PESQ_1</t>
+  </si>
+  <si>
+    <t>PESQ_2</t>
+  </si>
+  <si>
+    <t>Csig</t>
+  </si>
+  <si>
+    <t>Cbak</t>
+  </si>
+  <si>
+    <t>Covl</t>
+  </si>
+  <si>
+    <t>NCM</t>
+  </si>
+  <si>
+    <t>CSh</t>
+  </si>
+  <si>
+    <t>CSm</t>
+  </si>
+  <si>
+    <t>CSl</t>
+  </si>
+  <si>
+    <t>SII</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>mband_processed_output</t>
+  </si>
+  <si>
+    <t>python_mband_processed_output</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>mband_sp21_station_sn0.wav</t>
+  </si>
+  <si>
+    <t>mband_sp21_station_sn10.wav</t>
+  </si>
+  <si>
+    <t>mband_sp21_station_sn15.wav</t>
+  </si>
+  <si>
+    <t>mband_sp21_station_sn5.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn0.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn10.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn15.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn5.wav</t>
+  </si>
+  <si>
+    <t>SNR</t>
+  </si>
+  <si>
+    <t>SegSNR</t>
+  </si>
+  <si>
+    <t>WSS</t>
+  </si>
+  <si>
+    <t>LLR</t>
+  </si>
+  <si>
+    <t>IS</t>
+  </si>
+  <si>
+    <t>CEP</t>
+  </si>
+  <si>
+    <t>fwSNRseg</t>
+  </si>
+  <si>
+    <t>SIGv</t>
+  </si>
+  <si>
+    <t>BAKv</t>
+  </si>
+  <si>
+    <t>OVLv</t>
+  </si>
+  <si>
+    <t>SIGm</t>
+  </si>
+  <si>
+    <t>BAKm</t>
+  </si>
+  <si>
+    <t>OVLm</t>
+  </si>
+  <si>
+    <t>PESQ_1</t>
+  </si>
+  <si>
+    <t>PESQ_2</t>
+  </si>
+  <si>
+    <t>Csig</t>
+  </si>
+  <si>
+    <t>Cbak</t>
+  </si>
+  <si>
+    <t>Covl</t>
+  </si>
+  <si>
+    <t>NCM</t>
+  </si>
+  <si>
+    <t>CSh</t>
+  </si>
+  <si>
+    <t>CSm</t>
+  </si>
+  <si>
+    <t>CSl</t>
+  </si>
+  <si>
+    <t>SII</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>mband_processed_output</t>
+  </si>
+  <si>
+    <t>python_mband_processed_output</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>mband_sp21_station_sn0.wav</t>
+  </si>
+  <si>
+    <t>mband_sp21_station_sn10.wav</t>
+  </si>
+  <si>
+    <t>mband_sp21_station_sn15.wav</t>
+  </si>
+  <si>
+    <t>mband_sp21_station_sn5.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn0.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn10.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn15.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn5.wav</t>
+  </si>
+  <si>
+    <t>SNR</t>
+  </si>
+  <si>
+    <t>SegSNR</t>
+  </si>
+  <si>
+    <t>WSS</t>
+  </si>
+  <si>
+    <t>LLR</t>
+  </si>
+  <si>
+    <t>IS</t>
+  </si>
+  <si>
+    <t>CEP</t>
+  </si>
+  <si>
+    <t>fwSNRseg</t>
+  </si>
+  <si>
+    <t>SIGv</t>
+  </si>
+  <si>
+    <t>BAKv</t>
+  </si>
+  <si>
+    <t>OVLv</t>
+  </si>
+  <si>
+    <t>SIGm</t>
+  </si>
+  <si>
+    <t>BAKm</t>
+  </si>
+  <si>
+    <t>OVLm</t>
+  </si>
+  <si>
+    <t>PESQ_1</t>
+  </si>
+  <si>
+    <t>PESQ_2</t>
+  </si>
+  <si>
+    <t>Csig</t>
+  </si>
+  <si>
+    <t>Cbak</t>
+  </si>
+  <si>
+    <t>Covl</t>
+  </si>
+  <si>
+    <t>NCM</t>
+  </si>
+  <si>
+    <t>CSh</t>
+  </si>
+  <si>
+    <t>CSm</t>
+  </si>
+  <si>
+    <t>CSl</t>
+  </si>
+  <si>
+    <t>SII</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>mband_processed_output</t>
+  </si>
+  <si>
+    <t>python_mband_processed_output</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>mband_sp21_station_sn0.wav</t>
+  </si>
+  <si>
+    <t>mband_sp21_station_sn10.wav</t>
+  </si>
+  <si>
+    <t>mband_sp21_station_sn15.wav</t>
+  </si>
+  <si>
+    <t>mband_sp21_station_sn5.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn0.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn10.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn15.wav</t>
+  </si>
+  <si>
+    <t>python_mband_sp21_station_sn5.wav</t>
+  </si>
+  <si>
+    <t>SNR</t>
+  </si>
+  <si>
+    <t>SegSNR</t>
+  </si>
+  <si>
+    <t>WSS</t>
+  </si>
+  <si>
+    <t>LLR</t>
+  </si>
+  <si>
+    <t>IS</t>
+  </si>
+  <si>
+    <t>CEP</t>
+  </si>
+  <si>
+    <t>fwSNRseg</t>
+  </si>
+  <si>
+    <t>SIGv</t>
+  </si>
+  <si>
+    <t>BAKv</t>
+  </si>
+  <si>
+    <t>OVLv</t>
+  </si>
+  <si>
+    <t>SIGm</t>
+  </si>
+  <si>
+    <t>BAKm</t>
+  </si>
+  <si>
+    <t>OVLm</t>
+  </si>
+  <si>
+    <t>PESQ_1</t>
+  </si>
+  <si>
+    <t>PESQ_2</t>
+  </si>
+  <si>
+    <t>Csig</t>
+  </si>
+  <si>
+    <t>Cbak</t>
+  </si>
+  <si>
+    <t>Covl</t>
+  </si>
+  <si>
+    <t>NCM</t>
+  </si>
+  <si>
+    <t>CSh</t>
+  </si>
+  <si>
+    <t>CSm</t>
+  </si>
+  <si>
+    <t>CSl</t>
+  </si>
+  <si>
+    <t>SII</t>
+  </si>
   <si>
     <t>Algorithm</t>
   </si>
@@ -532,153 +1162,153 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>210</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>3</v>
+        <v>213</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>12</v>
+        <v>222</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>13</v>
+        <v>223</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>14</v>
+        <v>224</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>15</v>
+        <v>225</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>16</v>
+        <v>226</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>17</v>
+        <v>227</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>18</v>
+        <v>228</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>19</v>
+        <v>229</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>20</v>
+        <v>230</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>21</v>
+        <v>231</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>22</v>
+        <v>232</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>23</v>
+        <v>233</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>24</v>
+        <v>234</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>25</v>
+        <v>235</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>26</v>
+        <v>236</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>27</v>
+        <v>237</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>28</v>
+        <v>238</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>29</v>
+        <v>239</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>30</v>
+        <v>240</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>31</v>
+        <v>241</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>32</v>
+        <v>242</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>33</v>
+        <v>243</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>211</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>4</v>
+        <v>214</v>
       </c>
       <c r="C2" s="0">
-        <v>-10.206962587786265</v>
+        <v>-8.5485798740429075</v>
       </c>
       <c r="D2" s="0">
-        <v>-8.7632364591021208</v>
+        <v>-7.8186954769860115</v>
       </c>
       <c r="E2" s="0">
-        <v>80.383830439822262</v>
+        <v>76.115569507737561</v>
       </c>
       <c r="F2" s="0">
-        <v>1.0774613457300257</v>
+        <v>1.0637284526118578</v>
       </c>
       <c r="G2" s="0">
-        <v>4.3070076111146811</v>
+        <v>3.7012699802074374</v>
       </c>
       <c r="H2" s="0">
-        <v>6.0293571045889687</v>
+        <v>6.0933217976940091</v>
       </c>
       <c r="I2" s="0">
-        <v>6.1429092773455816</v>
+        <v>6.0503894393303073</v>
       </c>
       <c r="J2" s="0">
-        <v>2.4296842457941334</v>
+        <v>2.364772527758932</v>
       </c>
       <c r="K2" s="0">
-        <v>2.0364047570927508</v>
+        <v>2.0302092899651214</v>
       </c>
       <c r="L2" s="0">
-        <v>1.9628522693905692</v>
+        <v>1.9419944169125303</v>
       </c>
       <c r="M2" s="0">
-        <v>1.9796827468556308</v>
+        <v>2.1530192012362019</v>
       </c>
       <c r="N2" s="0">
-        <v>2.1781637527108497</v>
+        <v>2.090847134109556</v>
       </c>
       <c r="O2" s="0">
-        <v>1.9535190493745405</v>
+        <v>2.1658217118195751</v>
       </c>
       <c r="P2" s="0">
-        <v>1.8771836550370669</v>
+        <v>1.8761890347670953</v>
       </c>
       <c r="Q2" s="0">
-        <v>1.5400311126230202</v>
+        <v>1.5393360456542964</v>
       </c>
       <c r="R2" s="0">
-        <v>2.2692155783666998</v>
+        <v>2.3333275224678585</v>
       </c>
       <c r="S2" s="0">
-        <v>1.4165230771055284</v>
+        <v>1.5054315570143899</v>
       </c>
       <c r="T2" s="0">
-        <v>1.9293040407605118</v>
+        <v>1.97146598328208</v>
       </c>
       <c r="U2" s="0">
-        <v>0.55779137485575192</v>
+        <v>0.56268936636745548</v>
       </c>
       <c r="V2" s="0">
-        <v>0.63294303821523279</v>
+        <v>0.6502012509918863</v>
       </c>
       <c r="W2" s="0">
-        <v>0.36602415960328855</v>
+        <v>0.37607084722408091</v>
       </c>
       <c r="X2" s="0">
-        <v>0.047820163880449199</v>
+        <v>0.040314128773576173</v>
       </c>
       <c r="Y2" s="0">
         <v>0.23571173354711331</v>
@@ -686,76 +1316,76 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>1</v>
+        <v>211</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>5</v>
+        <v>215</v>
       </c>
       <c r="C3" s="0">
-        <v>-7.4920028083323125</v>
+        <v>-6.3772198878785193</v>
       </c>
       <c r="D3" s="0">
-        <v>-7.8958260986933926</v>
+        <v>-7.1241338228082833</v>
       </c>
       <c r="E3" s="0">
-        <v>56.276269303721904</v>
+        <v>51.26140278009035</v>
       </c>
       <c r="F3" s="0">
-        <v>0.55717475663864435</v>
+        <v>0.60674509297341872</v>
       </c>
       <c r="G3" s="0">
-        <v>2.1350521794214123</v>
+        <v>1.8198975576403746</v>
       </c>
       <c r="H3" s="0">
-        <v>4.060070898026269</v>
+        <v>4.2944577880489367</v>
       </c>
       <c r="I3" s="0">
-        <v>11.002920887378444</v>
+        <v>10.517490430560629</v>
       </c>
       <c r="J3" s="0">
-        <v>4.3895344364072608</v>
+        <v>3.9581710288706606</v>
       </c>
       <c r="K3" s="0">
-        <v>2.7631765150699215</v>
+        <v>2.8901025888258571</v>
       </c>
       <c r="L3" s="0">
-        <v>3.5060319162816955</v>
+        <v>3.3218757092161066</v>
       </c>
       <c r="M3" s="0">
-        <v>3.8296044289359532</v>
+        <v>3.9149568210124843</v>
       </c>
       <c r="N3" s="0">
-        <v>3.009822587000814</v>
+        <v>3.450985516073886</v>
       </c>
       <c r="O3" s="0">
-        <v>3.4441373781592137</v>
+        <v>3.4846402687314999</v>
       </c>
       <c r="P3" s="0">
-        <v>2.6152208136249246</v>
+        <v>2.601772396032449</v>
       </c>
       <c r="Q3" s="0">
-        <v>2.2803227674681681</v>
+        <v>2.2628828960183851</v>
       </c>
       <c r="R3" s="0">
-        <v>3.590156149332298</v>
+        <v>3.574492909694881</v>
       </c>
       <c r="S3" s="0">
-        <v>1.9927046195689764</v>
+        <v>2.0699969550059567</v>
       </c>
       <c r="T3" s="0">
-        <v>3.020044024647047</v>
+        <v>3.0181062997856847</v>
       </c>
       <c r="U3" s="0">
-        <v>0.89511970232695648</v>
+        <v>0.90158334739209689</v>
       </c>
       <c r="V3" s="0">
-        <v>0.93274279767632406</v>
+        <v>0.90841098611064308</v>
       </c>
       <c r="W3" s="0">
-        <v>0.69310217467735336</v>
+        <v>0.68496878593128507</v>
       </c>
       <c r="X3" s="0">
-        <v>0.22644291856792953</v>
+        <v>0.20817752525871697</v>
       </c>
       <c r="Y3" s="0">
         <v>0.23571173354711331</v>
@@ -763,76 +1393,76 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>1</v>
+        <v>211</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>6</v>
+        <v>216</v>
       </c>
       <c r="C4" s="0">
-        <v>-7.0988077885401148</v>
+        <v>-6.0382867568486684</v>
       </c>
       <c r="D4" s="0">
-        <v>-7.0983677765694786</v>
+        <v>-6.5129714901912914</v>
       </c>
       <c r="E4" s="0">
-        <v>40.725819242441403</v>
+        <v>40.359746677123141</v>
       </c>
       <c r="F4" s="0">
-        <v>0.40229757303201485</v>
+        <v>0.42506162981666107</v>
       </c>
       <c r="G4" s="0">
-        <v>1.4532672881397013</v>
+        <v>1.4661518813452556</v>
       </c>
       <c r="H4" s="0">
-        <v>3.2756878352647587</v>
+        <v>3.4682183225852263</v>
       </c>
       <c r="I4" s="0">
-        <v>12.851029913116449</v>
+        <v>12.03598930935105</v>
       </c>
       <c r="J4" s="0">
-        <v>4.6490308268226981</v>
+        <v>4.1648031588382786</v>
       </c>
       <c r="K4" s="0">
-        <v>3.0183892412638982</v>
+        <v>2.9484716317121284</v>
       </c>
       <c r="L4" s="0">
-        <v>3.770397652546162</v>
+        <v>3.4617709445197717</v>
       </c>
       <c r="M4" s="0">
-        <v>3.5604553026326329</v>
+        <v>3.8307356378113382</v>
       </c>
       <c r="N4" s="0">
-        <v>1.5382947017664645</v>
+        <v>1.4533504735832592</v>
       </c>
       <c r="O4" s="0">
-        <v>4.1017506483269415</v>
+        <v>3.8113180359322367</v>
       </c>
       <c r="P4" s="0">
-        <v>3.0112614726900464</v>
+        <v>2.9820199420242166</v>
       </c>
       <c r="Q4" s="0">
-        <v>2.838973094345131</v>
+        <v>2.7956340793634826</v>
       </c>
       <c r="R4" s="0">
-        <v>4.1282940922001821</v>
+        <v>4.0905318878651498</v>
       </c>
       <c r="S4" s="0">
-        <v>2.3411050793248749</v>
+        <v>2.366570101665662</v>
       </c>
       <c r="T4" s="0">
-        <v>3.5270083934260059</v>
+        <v>3.4943762721235014</v>
       </c>
       <c r="U4" s="0">
-        <v>0.94336477866728841</v>
+        <v>0.93748530750150627</v>
       </c>
       <c r="V4" s="0">
-        <v>0.98303586609633664</v>
+        <v>0.95337751966252382</v>
       </c>
       <c r="W4" s="0">
-        <v>0.85278164553633851</v>
+        <v>0.82497581497185257</v>
       </c>
       <c r="X4" s="0">
-        <v>0.30246232820655033</v>
+        <v>0.28214594634898915</v>
       </c>
       <c r="Y4" s="0">
         <v>0.23571173354711331</v>
@@ -840,76 +1470,76 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>1</v>
+        <v>211</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>7</v>
+        <v>217</v>
       </c>
       <c r="C5" s="0">
-        <v>-9.1155293751566155</v>
+        <v>-8.025338879250711</v>
       </c>
       <c r="D5" s="0">
-        <v>-8.8648797560871735</v>
+        <v>-8.4549570367357632</v>
       </c>
       <c r="E5" s="0">
-        <v>58.720542706425235</v>
+        <v>59.087109840062261</v>
       </c>
       <c r="F5" s="0">
-        <v>0.7249952104412537</v>
+        <v>0.77350611996255514</v>
       </c>
       <c r="G5" s="0">
-        <v>2.9412518374919721</v>
+        <v>2.716537229351538</v>
       </c>
       <c r="H5" s="0">
-        <v>4.9929053340945995</v>
+        <v>5.1631338718877746</v>
       </c>
       <c r="I5" s="0">
-        <v>8.6172338883876449</v>
+        <v>8.2342659036933163</v>
       </c>
       <c r="J5" s="0">
-        <v>3.994858507289675</v>
+        <v>3.6560280516966834</v>
       </c>
       <c r="K5" s="0">
-        <v>2.4224201164402768</v>
+        <v>2.2935280482498976</v>
       </c>
       <c r="L5" s="0">
-        <v>3.1216152348072068</v>
+        <v>2.8615516141641204</v>
       </c>
       <c r="M5" s="0">
-        <v>3.2813624654715969</v>
+        <v>3.4292117573950893</v>
       </c>
       <c r="N5" s="0">
-        <v>2.6421734865610143</v>
+        <v>2.8938529170377203</v>
       </c>
       <c r="O5" s="0">
-        <v>2.7223095967364173</v>
+        <v>2.8330499803292888</v>
       </c>
       <c r="P5" s="0">
-        <v>2.4369790533194928</v>
+        <v>2.4443287998607275</v>
       </c>
       <c r="Q5" s="0">
-        <v>2.0601736371841146</v>
+        <v>2.0687595282970013</v>
       </c>
       <c r="R5" s="0">
-        <v>3.2742951051865758</v>
+        <v>3.223107946956616</v>
       </c>
       <c r="S5" s="0">
-        <v>1.829344763908249</v>
+        <v>1.8561171041386388</v>
       </c>
       <c r="T5" s="0">
-        <v>2.7667109178315274</v>
+        <v>2.7440286318500084</v>
       </c>
       <c r="U5" s="0">
-        <v>0.77154919263139143</v>
+        <v>0.77316881333802945</v>
       </c>
       <c r="V5" s="0">
-        <v>0.83653851376018207</v>
+        <v>0.81599283138694234</v>
       </c>
       <c r="W5" s="0">
-        <v>0.56994932531555342</v>
+        <v>0.57099320667547016</v>
       </c>
       <c r="X5" s="0">
-        <v>0.16371209276939594</v>
+        <v>0.16026574709830702</v>
       </c>
       <c r="Y5" s="0">
         <v>0.23571173354711331</v>
@@ -917,10 +1547,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>2</v>
+        <v>212</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>8</v>
+        <v>218</v>
       </c>
       <c r="C6" s="0">
         <v>-5.4256534416546103</v>
@@ -994,10 +1624,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>2</v>
+        <v>212</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>9</v>
+        <v>219</v>
       </c>
       <c r="C7" s="0">
         <v>-2.2829037278246589</v>
@@ -1071,10 +1701,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>2</v>
+        <v>212</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>10</v>
+        <v>220</v>
       </c>
       <c r="C8" s="0">
         <v>-1.6799527745454543</v>
@@ -1148,10 +1778,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>2</v>
+        <v>212</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>11</v>
+        <v>221</v>
       </c>
       <c r="C9" s="0">
         <v>-4.4471840550030661</v>

</xml_diff>